<commit_message>
VISTA-2237  Preload data/(tenants + applications) for Generic Test Cases - iDecision of Equifax
</commit_message>
<xml_diff>
--- a/vista-dev/vista-dev-generator/src/main/resources/com/propertyvista/generator/iDecision-GenericTestCases.xlsx
+++ b/vista-dev/vista-dev-generator/src/main/resources/com/propertyvista/generator/iDecision-GenericTestCases.xlsx
@@ -8,11 +8,9 @@
   </bookViews>
   <sheets>
     <sheet name="iDecision - test cases" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'iDecision - test cases'!$B$1:$N$20</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'iDecision - test cases'!$B$1:$N$19</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -692,14 +690,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -1005,7 +996,7 @@
   <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B6" sqref="A1:XFD6"/>
+      <selection activeCell="B19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.33203125" defaultRowHeight="18.75" customHeight="1"/>
@@ -1864,41 +1855,12 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G4:K18">
-    <cfRule type="expression" dxfId="1" priority="8">
-      <formula>#REF!=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G19:K19">
-    <cfRule type="expression" dxfId="0" priority="1">
+  <conditionalFormatting sqref="G4:K19">
+    <cfRule type="expression" dxfId="0" priority="8">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>